<commit_message>
add persons in cmip6_cmcc_cmcc-cm2-sr5_seaice
</commit_message>
<xml_diff>
--- a/cmip6/models/cmcc-cm2-sr5/cmip6_cmcc_cmcc-cm2-sr5_seaice.xlsx
+++ b/cmip6/models/cmcc-cm2-sr5/cmip6_cmcc_cmcc-cm2-sr5_seaice.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lovato/GIT/ES-DOC-INST-cmcc/cmip6/models/cmcc-cm2-sr5/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC349901-B595-9D40-86AA-89EC9C3A409E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBB0D9DB-4290-1745-9944-290677509289}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="100" yWindow="460" windowWidth="25500" windowHeight="14180" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="100" yWindow="460" windowWidth="25500" windowHeight="14180" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Frontis" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="869" uniqueCount="567">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="873" uniqueCount="571">
   <si>
     <t>ES-DOC CMIP6 Model Documentation</t>
   </si>
@@ -1748,6 +1748,18 @@
   </si>
   <si>
     <t>assur_1958</t>
+  </si>
+  <si>
+    <t>IOVINO-DOROTEACIRO</t>
+  </si>
+  <si>
+    <t>Principal Investigator</t>
+  </si>
+  <si>
+    <t>FOGLI-PIER-GIUSEPPE</t>
+  </si>
+  <si>
+    <t>Contributor</t>
   </si>
 </sst>
 </file>
@@ -2284,7 +2296,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
@@ -2417,10 +2429,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView zoomScale="99" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" zoomScale="99" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2473,82 +2485,98 @@
         <v>565</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A12" s="9" t="s">
+    <row r="10" spans="1:2" ht="19" x14ac:dyDescent="0.2">
+      <c r="A10" s="11" t="s">
+        <v>567</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="19" x14ac:dyDescent="0.2">
+      <c r="A11" s="11" t="s">
+        <v>569</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A14" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="B12" s="9"/>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="8" t="s">
-        <v>33</v>
-      </c>
+      <c r="B14" s="9"/>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="8" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" s="10" t="s">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="10" t="s">
+      <c r="B18" s="10" t="s">
         <v>35</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="19" x14ac:dyDescent="0.2">
-      <c r="A17" s="11" t="s">
-        <v>549</v>
-      </c>
-      <c r="B17" s="11" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="19" x14ac:dyDescent="0.2">
-      <c r="A18" s="11" t="s">
-        <v>566</v>
-      </c>
-      <c r="B18" s="11" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="19" x14ac:dyDescent="0.2">
       <c r="A19" s="11" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>288</v>
+        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="19" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
-        <v>554</v>
+        <v>566</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>288</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="19" x14ac:dyDescent="0.2">
       <c r="A21" s="11" t="s">
+        <v>553</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="19" x14ac:dyDescent="0.2">
+      <c r="A22" s="11" t="s">
+        <v>554</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="19" x14ac:dyDescent="0.2">
+      <c r="A23" s="11" t="s">
         <v>551</v>
       </c>
-      <c r="B21" s="11" t="s">
+      <c r="B23" s="11" t="s">
         <v>511</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9:B11" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"Author,Contributor,Principal Investigator,Point of Contact,Sponsor"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B17:B21" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B19:B23" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>"Top Level,Key Properties,Grid,Dynamics,Thermodynamics,Radiative Processes"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="A6" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="A13" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="A15" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2558,8 +2586,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AL156"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="87" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView topLeftCell="A38" zoomScale="87" workbookViewId="0">
+      <selection activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>